<commit_message>
added ideas and better plots
</commit_message>
<xml_diff>
--- a/data/zerforschen_green_tea_effect.xlsx
+++ b/data/zerforschen_green_tea_effect.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kruppajo/work/GitHub/jkruppa.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3CEB29-8702-7D40-A391-7EEEF9A67DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209AE391-3122-244E-841F-701565850BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2420" yWindow="4460" windowWidth="15440" windowHeight="13620" xr2:uid="{7CBCB879-B308-034B-BADE-92757FC3BFA5}"/>
   </bookViews>
@@ -44,10 +44,10 @@
     <t>trt</t>
   </si>
   <si>
-    <t>GTE</t>
+    <t>PLA</t>
   </si>
   <si>
-    <t>Placebo</t>
+    <t>GTE</t>
   </si>
   <si>
     <t>fat_ox_r_kj_min</t>
@@ -425,7 +425,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -449,7 +449,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>4.4000000000000004</v>
@@ -460,7 +460,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>4.0999999999999996</v>
@@ -471,7 +471,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>3.8</v>
@@ -482,7 +482,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>5.6</v>
@@ -493,7 +493,7 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <v>5.0999999999999996</v>
@@ -504,7 +504,7 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <v>4.5999999999999996</v>
@@ -515,7 +515,7 @@
         <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <v>6</v>
@@ -526,7 +526,7 @@
         <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <v>5.6</v>
@@ -537,7 +537,7 @@
         <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>5.2</v>
@@ -548,7 +548,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <v>5.2</v>
@@ -559,7 +559,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12">
         <v>4.8</v>
@@ -570,7 +570,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13">
         <v>4.4000000000000004</v>
@@ -581,7 +581,7 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C14">
         <v>6.3</v>
@@ -592,7 +592,7 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15">
         <v>5.8</v>
@@ -603,7 +603,7 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16">
         <v>5.3</v>
@@ -614,7 +614,7 @@
         <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17">
         <v>6.9</v>
@@ -625,7 +625,7 @@
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C18">
         <v>6.6</v>
@@ -636,7 +636,7 @@
         <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C19">
         <v>6.3</v>

</xml_diff>